<commit_message>
Additional refactoring of arg commands bugs
</commit_message>
<xml_diff>
--- a/classification_report_inference_model.xlsx
+++ b/classification_report_inference_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nsq024vs\u8\aczd087\MyDocs\GLCM_svm_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D51D3A-9268-4422-9702-A9970D2DEDE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AE03DA-5DB0-4E76-BBDD-755E19ACE622}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="168">
   <si>
     <t>background</t>
   </si>
@@ -925,15 +925,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L162"/>
+  <dimension ref="A1:M162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -953,19 +953,22 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -988,23 +991,27 @@
         <v>0</v>
       </c>
       <c r="I2">
+        <f>AVERAGE(B2:B162)</f>
+        <v>0.962045406367526</v>
+      </c>
+      <c r="J2">
         <f>AVERAGE(D2:D162)</f>
         <v>7.1418924207867661E-4</v>
       </c>
-      <c r="J2">
-        <f t="shared" ref="J2:L2" si="0">AVERAGE(E2:E162)</f>
+      <c r="K2">
+        <f>AVERAGE(E2:E162)</f>
         <v>0.1963717815247934</v>
       </c>
-      <c r="K2">
-        <f t="shared" si="0"/>
+      <c r="L2">
+        <f>AVERAGE(F2:F162)</f>
         <v>5.9890364696902412E-3</v>
       </c>
-      <c r="L2">
-        <f t="shared" si="0"/>
+      <c r="M2">
+        <f>AVERAGE(G2:G162)</f>
         <v>5.8916848031248678E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1027,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1050,7 +1057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1073,7 +1080,7 @@
         <v>2.5316455696202531E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1096,7 +1103,7 @@
         <v>7.9412746079412747E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1119,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1142,7 +1149,7 @@
         <v>0.16826003824091779</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1165,7 +1172,7 @@
         <v>3.6574487065120419E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1188,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1211,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1234,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1257,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1280,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1303,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>

</xml_diff>